<commit_message>
Update reports to specify create timestamp is UTC
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Action_Required_Template.xlsx
+++ b/app/server/static/templates/reports/Action_Required_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://parcsystems.sharepoint.com/projects/Shared Documents/MALS/CDOGS/Development/MALS_Templates/Reports/Action_Required/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{86A9A722-797B-2542-95DF-8D89800B15B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6F3CDA80-C107-5C4D-A733-737455AB4086}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA734FF-32F7-4357-8ABB-3D726EE0BCFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19100" yWindow="-16740" windowWidth="26320" windowHeight="12120" xr2:uid="{6889C3E9-B59E-5546-B2AA-D5CBDE858824}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6889C3E9-B59E-5546-B2AA-D5CBDE858824}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Action Required Report</t>
   </si>
   <si>
-    <t>Date &amp; Time Report Created</t>
-  </si>
-  <si>
     <t>Status:</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>{d.RowCount}</t>
+  </si>
+  <si>
+    <t>Date &amp; Time Report Created (UTC)</t>
   </si>
 </sst>
 </file>
@@ -204,15 +204,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>88900</xdr:colOff>
+          <xdr:colOff>85725</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>596900</xdr:colOff>
+          <xdr:colOff>600075</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>573947</xdr:rowOff>
+          <xdr:rowOff>581025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -222,7 +222,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{471CA4BF-FDA9-624C-8194-DCA3B81C641C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -557,52 +557,52 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -610,75 +610,75 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -693,15 +693,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>88900</xdr:colOff>
+                <xdr:colOff>85725</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>596900</xdr:colOff>
+                <xdr:colOff>600075</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>584200</xdr:rowOff>
+                <xdr:rowOff>581025</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -716,18 +716,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -942,6 +942,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2722AF27-64EF-4127-A9ED-AB98770F6FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741B16B2-29F6-48D6-A1A6-4987DCE172D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
@@ -954,14 +962,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2722AF27-64EF-4127-A9ED-AB98770F6FD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>